<commit_message>
add RKI data downloaded 2020-11-30--13-35-01
</commit_message>
<xml_diff>
--- a/rki-data/RKI-COVID-19_Todesfaelle.xlsx
+++ b/rki-data/RKI-COVID-19_Todesfaelle.xlsx
@@ -7,13 +7,14 @@
   </bookViews>
   <sheets>
     <sheet name="COVID_Todesfälle" sheetId="1" r:id="rId2"/>
+    <sheet name="COVID_Todesfälle_Monat" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
   <si>
     <t>Sterbewoche</t>
   </si>
@@ -33,28 +34,28 @@
     <t>162</t>
   </si>
   <si>
-    <t>601</t>
-  </si>
-  <si>
-    <t>1367</t>
-  </si>
-  <si>
-    <t>1738</t>
+    <t>600</t>
+  </si>
+  <si>
+    <t>1368</t>
+  </si>
+  <si>
+    <t>1741</t>
   </si>
   <si>
     <t>1594</t>
   </si>
   <si>
-    <t>1166</t>
-  </si>
-  <si>
-    <t>781</t>
-  </si>
-  <si>
-    <t>511</t>
-  </si>
-  <si>
-    <t>348</t>
+    <t>1168</t>
+  </si>
+  <si>
+    <t>782</t>
+  </si>
+  <si>
+    <t>512</t>
+  </si>
+  <si>
+    <t>350</t>
   </si>
   <si>
     <t>270</t>
@@ -72,43 +73,79 @@
     <t>47</t>
   </si>
   <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
     <t>50</t>
   </si>
   <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
     <t>65</t>
   </si>
   <si>
-    <t>77</t>
+    <t>78</t>
+  </si>
+  <si>
+    <t>112</t>
+  </si>
+  <si>
+    <t>216</t>
+  </si>
+  <si>
+    <t>363</t>
+  </si>
+  <si>
+    <t>687</t>
+  </si>
+  <si>
+    <t>SterbeMonat</t>
+  </si>
+  <si>
+    <t>1118</t>
+  </si>
+  <si>
+    <t>6040</t>
+  </si>
+  <si>
+    <t>1558</t>
+  </si>
+  <si>
+    <t>302</t>
+  </si>
+  <si>
+    <t>131</t>
+  </si>
+  <si>
+    <t>143</t>
+  </si>
+  <si>
+    <t>196</t>
+  </si>
+  <si>
+    <t>1312</t>
   </si>
 </sst>
 </file>
@@ -152,7 +189,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B45"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -392,7 +429,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31">
@@ -400,7 +437,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32">
@@ -408,7 +445,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33">
@@ -416,7 +453,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34">
@@ -424,7 +461,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35">
@@ -432,7 +469,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36">
@@ -440,7 +477,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37">
@@ -448,7 +485,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38">
@@ -464,7 +501,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40">
@@ -472,7 +509,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41">
@@ -480,7 +517,120 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B9"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add RKI data downloaded 2020-12-15--13-35-01
</commit_message>
<xml_diff>
--- a/rki-data/RKI-COVID-19_Todesfaelle.xlsx
+++ b/rki-data/RKI-COVID-19_Todesfaelle.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
   <si>
     <t>Sterbewoche</t>
   </si>
@@ -40,7 +40,7 @@
     <t>1368</t>
   </si>
   <si>
-    <t>1741</t>
+    <t>1740</t>
   </si>
   <si>
     <t>1594</t>
@@ -49,25 +49,25 @@
     <t>1168</t>
   </si>
   <si>
-    <t>782</t>
-  </si>
-  <si>
-    <t>512</t>
-  </si>
-  <si>
-    <t>350</t>
-  </si>
-  <si>
-    <t>270</t>
+    <t>783</t>
+  </si>
+  <si>
+    <t>514</t>
+  </si>
+  <si>
+    <t>351</t>
+  </si>
+  <si>
+    <t>271</t>
   </si>
   <si>
     <t>150</t>
   </si>
   <si>
-    <t>113</t>
-  </si>
-  <si>
-    <t>72</t>
+    <t>112</t>
+  </si>
+  <si>
+    <t>73</t>
   </si>
   <si>
     <t>47</t>
@@ -91,6 +91,9 @@
     <t>30</t>
   </si>
   <si>
+    <t>32</t>
+  </si>
+  <si>
     <t>37</t>
   </si>
   <si>
@@ -100,7 +103,7 @@
     <t>19</t>
   </si>
   <si>
-    <t>50</t>
+    <t>52</t>
   </si>
   <si>
     <t>65</t>
@@ -109,28 +112,34 @@
     <t>78</t>
   </si>
   <si>
-    <t>112</t>
-  </si>
-  <si>
-    <t>216</t>
-  </si>
-  <si>
-    <t>363</t>
-  </si>
-  <si>
-    <t>687</t>
+    <t>115</t>
+  </si>
+  <si>
+    <t>226</t>
+  </si>
+  <si>
+    <t>378</t>
+  </si>
+  <si>
+    <t>725</t>
+  </si>
+  <si>
+    <t>1105</t>
+  </si>
+  <si>
+    <t>1455</t>
   </si>
   <si>
     <t>SterbeMonat</t>
   </si>
   <si>
-    <t>1118</t>
-  </si>
-  <si>
-    <t>6040</t>
-  </si>
-  <si>
-    <t>1558</t>
+    <t>1117</t>
+  </si>
+  <si>
+    <t>6041</t>
+  </si>
+  <si>
+    <t>1562</t>
   </si>
   <si>
     <t>302</t>
@@ -139,13 +148,16 @@
     <t>131</t>
   </si>
   <si>
-    <t>143</t>
-  </si>
-  <si>
-    <t>196</t>
-  </si>
-  <si>
-    <t>1312</t>
+    <t>145</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>1366</t>
+  </si>
+  <si>
+    <t>2682</t>
   </si>
 </sst>
 </file>
@@ -189,7 +201,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B47"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -229,7 +241,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -461,7 +473,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35">
@@ -469,7 +481,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36">
@@ -477,7 +489,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37">
@@ -485,7 +497,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38">
@@ -493,7 +505,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39">
@@ -501,7 +513,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="40">
@@ -509,7 +521,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41">
@@ -517,7 +529,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="42">
@@ -525,7 +537,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="43">
@@ -533,7 +545,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44">
@@ -541,7 +553,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45">
@@ -549,7 +561,23 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -558,12 +586,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -574,7 +602,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3">
@@ -582,7 +610,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4">
@@ -590,7 +618,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5">
@@ -598,7 +626,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6">
@@ -606,7 +634,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7">
@@ -614,7 +642,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8">
@@ -622,7 +650,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9">
@@ -630,7 +658,15 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add RKI data downloaded 2020-12-21--13-35-01
</commit_message>
<xml_diff>
--- a/rki-data/RKI-COVID-19_Todesfaelle.xlsx
+++ b/rki-data/RKI-COVID-19_Todesfaelle.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
   <si>
     <t>Sterbewoche</t>
   </si>
@@ -28,16 +28,16 @@
     <t>&lt;4</t>
   </si>
   <si>
-    <t>17</t>
+    <t>18</t>
   </si>
   <si>
     <t>162</t>
   </si>
   <si>
-    <t>600</t>
-  </si>
-  <si>
-    <t>1368</t>
+    <t>601</t>
+  </si>
+  <si>
+    <t>1369</t>
   </si>
   <si>
     <t>1740</t>
@@ -49,7 +49,7 @@
     <t>1168</t>
   </si>
   <si>
-    <t>783</t>
+    <t>782</t>
   </si>
   <si>
     <t>514</t>
@@ -85,55 +85,58 @@
     <t>31</t>
   </si>
   <si>
+    <t>30</t>
+  </si>
+  <si>
     <t>29</t>
   </si>
   <si>
-    <t>30</t>
-  </si>
-  <si>
     <t>32</t>
   </si>
   <si>
+    <t>39</t>
+  </si>
+  <si>
     <t>37</t>
   </si>
   <si>
-    <t>36</t>
-  </si>
-  <si>
     <t>19</t>
   </si>
   <si>
-    <t>52</t>
+    <t>53</t>
   </si>
   <si>
     <t>65</t>
   </si>
   <si>
-    <t>78</t>
-  </si>
-  <si>
-    <t>115</t>
-  </si>
-  <si>
-    <t>226</t>
-  </si>
-  <si>
-    <t>378</t>
-  </si>
-  <si>
-    <t>725</t>
-  </si>
-  <si>
-    <t>1105</t>
-  </si>
-  <si>
-    <t>1455</t>
+    <t>79</t>
+  </si>
+  <si>
+    <t>116</t>
+  </si>
+  <si>
+    <t>230</t>
+  </si>
+  <si>
+    <t>387</t>
+  </si>
+  <si>
+    <t>746</t>
+  </si>
+  <si>
+    <t>1134</t>
+  </si>
+  <si>
+    <t>1497</t>
+  </si>
+  <si>
+    <t>1887</t>
   </si>
   <si>
     <t>SterbeMonat</t>
   </si>
   <si>
-    <t>1117</t>
+    <t>1119</t>
   </si>
   <si>
     <t>6041</t>
@@ -148,16 +151,16 @@
     <t>131</t>
   </si>
   <si>
-    <t>145</t>
-  </si>
-  <si>
-    <t>200</t>
-  </si>
-  <si>
-    <t>1366</t>
-  </si>
-  <si>
-    <t>2682</t>
+    <t>148</t>
+  </si>
+  <si>
+    <t>201</t>
+  </si>
+  <si>
+    <t>1398</t>
+  </si>
+  <si>
+    <t>4644</t>
   </si>
 </sst>
 </file>
@@ -201,7 +204,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B47"/>
+  <dimension ref="A1:B49"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -225,28 +228,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -254,15 +257,15 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
@@ -270,7 +273,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
@@ -278,7 +281,7 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
@@ -286,159 +289,159 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
         <v>21</v>
@@ -446,138 +449,154 @@
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0">
         <v>46</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -591,7 +610,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -602,7 +621,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3">
@@ -610,7 +629,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4">
@@ -618,7 +637,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5">
@@ -626,7 +645,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6">
@@ -634,7 +653,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7">
@@ -642,7 +661,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8">
@@ -650,7 +669,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9">
@@ -658,7 +677,7 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10">
@@ -666,7 +685,7 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add RKI data downloaded 2020-12-29--13-35-01
</commit_message>
<xml_diff>
--- a/rki-data/RKI-COVID-19_Todesfaelle.xlsx
+++ b/rki-data/RKI-COVID-19_Todesfaelle.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
   <si>
     <t>Sterbewoche</t>
   </si>
@@ -43,31 +43,31 @@
     <t>1740</t>
   </si>
   <si>
-    <t>1594</t>
-  </si>
-  <si>
-    <t>1168</t>
-  </si>
-  <si>
-    <t>782</t>
-  </si>
-  <si>
-    <t>514</t>
-  </si>
-  <si>
-    <t>351</t>
-  </si>
-  <si>
-    <t>271</t>
+    <t>1598</t>
+  </si>
+  <si>
+    <t>1170</t>
+  </si>
+  <si>
+    <t>783</t>
+  </si>
+  <si>
+    <t>515</t>
+  </si>
+  <si>
+    <t>352</t>
+  </si>
+  <si>
+    <t>272</t>
   </si>
   <si>
     <t>150</t>
   </si>
   <si>
-    <t>112</t>
-  </si>
-  <si>
-    <t>73</t>
+    <t>113</t>
+  </si>
+  <si>
+    <t>72</t>
   </si>
   <si>
     <t>47</t>
@@ -79,15 +79,15 @@
     <t>46</t>
   </si>
   <si>
+    <t>27</t>
+  </si>
+  <si>
     <t>26</t>
   </si>
   <si>
     <t>31</t>
   </si>
   <si>
-    <t>30</t>
-  </si>
-  <si>
     <t>29</t>
   </si>
   <si>
@@ -103,7 +103,7 @@
     <t>19</t>
   </si>
   <si>
-    <t>53</t>
+    <t>54</t>
   </si>
   <si>
     <t>65</t>
@@ -112,25 +112,28 @@
     <t>79</t>
   </si>
   <si>
-    <t>116</t>
-  </si>
-  <si>
-    <t>230</t>
-  </si>
-  <si>
-    <t>387</t>
-  </si>
-  <si>
-    <t>746</t>
-  </si>
-  <si>
-    <t>1134</t>
-  </si>
-  <si>
-    <t>1497</t>
-  </si>
-  <si>
-    <t>1887</t>
+    <t>117</t>
+  </si>
+  <si>
+    <t>232</t>
+  </si>
+  <si>
+    <t>389</t>
+  </si>
+  <si>
+    <t>756</t>
+  </si>
+  <si>
+    <t>1158</t>
+  </si>
+  <si>
+    <t>1527</t>
+  </si>
+  <si>
+    <t>1940</t>
+  </si>
+  <si>
+    <t>2579</t>
   </si>
   <si>
     <t>SterbeMonat</t>
@@ -139,28 +142,28 @@
     <t>1119</t>
   </si>
   <si>
-    <t>6041</t>
-  </si>
-  <si>
-    <t>1562</t>
+    <t>6048</t>
+  </si>
+  <si>
+    <t>1565</t>
   </si>
   <si>
     <t>302</t>
   </si>
   <si>
-    <t>131</t>
-  </si>
-  <si>
-    <t>148</t>
-  </si>
-  <si>
-    <t>201</t>
-  </si>
-  <si>
-    <t>1398</t>
-  </si>
-  <si>
-    <t>4644</t>
+    <t>132</t>
+  </si>
+  <si>
+    <t>147</t>
+  </si>
+  <si>
+    <t>202</t>
+  </si>
+  <si>
+    <t>1407</t>
+  </si>
+  <si>
+    <t>7335</t>
   </si>
 </sst>
 </file>
@@ -204,7 +207,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B50"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -276,7 +279,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
@@ -284,7 +287,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
@@ -452,7 +455,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32">
@@ -460,7 +463,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33">
@@ -468,7 +471,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34">
@@ -597,6 +600,14 @@
       </c>
       <c r="B49" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -605,12 +616,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -618,15 +629,15 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>41</v>
@@ -634,7 +645,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>42</v>
@@ -642,7 +653,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>43</v>
@@ -650,7 +661,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>44</v>
@@ -658,7 +669,7 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>45</v>
@@ -666,7 +677,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>46</v>
@@ -674,7 +685,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
         <v>47</v>
@@ -682,10 +693,18 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add RKI data downloaded 2021-01-01--13-35-01
</commit_message>
<xml_diff>
--- a/rki-data/RKI-COVID-19_Todesfaelle.xlsx
+++ b/rki-data/RKI-COVID-19_Todesfaelle.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
   <si>
     <t>Sterbewoche</t>
   </si>
@@ -34,16 +34,16 @@
     <t>162</t>
   </si>
   <si>
-    <t>601</t>
-  </si>
-  <si>
-    <t>1369</t>
+    <t>603</t>
+  </si>
+  <si>
+    <t>1371</t>
   </si>
   <si>
     <t>1740</t>
   </si>
   <si>
-    <t>1598</t>
+    <t>1597</t>
   </si>
   <si>
     <t>1170</t>
@@ -52,16 +52,16 @@
     <t>783</t>
   </si>
   <si>
-    <t>515</t>
-  </si>
-  <si>
-    <t>352</t>
-  </si>
-  <si>
-    <t>272</t>
-  </si>
-  <si>
-    <t>150</t>
+    <t>516</t>
+  </si>
+  <si>
+    <t>354</t>
+  </si>
+  <si>
+    <t>273</t>
+  </si>
+  <si>
+    <t>151</t>
   </si>
   <si>
     <t>113</t>
@@ -70,7 +70,7 @@
     <t>72</t>
   </si>
   <si>
-    <t>47</t>
+    <t>48</t>
   </si>
   <si>
     <t>51</t>
@@ -118,37 +118,37 @@
     <t>232</t>
   </si>
   <si>
-    <t>389</t>
-  </si>
-  <si>
-    <t>756</t>
-  </si>
-  <si>
-    <t>1158</t>
-  </si>
-  <si>
-    <t>1527</t>
-  </si>
-  <si>
-    <t>1940</t>
-  </si>
-  <si>
-    <t>2579</t>
+    <t>390</t>
+  </si>
+  <si>
+    <t>757</t>
+  </si>
+  <si>
+    <t>1548</t>
+  </si>
+  <si>
+    <t>1965</t>
+  </si>
+  <si>
+    <t>2606</t>
+  </si>
+  <si>
+    <t>2919</t>
   </si>
   <si>
     <t>SterbeMonat</t>
   </si>
   <si>
-    <t>1119</t>
-  </si>
-  <si>
-    <t>6048</t>
-  </si>
-  <si>
-    <t>1565</t>
-  </si>
-  <si>
-    <t>302</t>
+    <t>1122</t>
+  </si>
+  <si>
+    <t>6049</t>
+  </si>
+  <si>
+    <t>1569</t>
+  </si>
+  <si>
+    <t>303</t>
   </si>
   <si>
     <t>132</t>
@@ -160,10 +160,10 @@
     <t>202</t>
   </si>
   <si>
-    <t>1407</t>
-  </si>
-  <si>
-    <t>7335</t>
+    <t>1410</t>
+  </si>
+  <si>
+    <t>7837</t>
   </si>
 </sst>
 </file>
@@ -207,7 +207,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:B51"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -255,7 +255,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -583,7 +583,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48">
@@ -591,7 +591,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="49">
@@ -599,7 +599,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="50">
@@ -607,6 +607,14 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>